<commit_message>
ejercicios 15 al 30 python
</commit_message>
<xml_diff>
--- a/retoPYTHON/ejercicios/100_ejercicios_python_para_ingeniero_datos.xlsx
+++ b/retoPYTHON/ejercicios/100_ejercicios_python_para_ingeniero_datos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DILZA RAMIREZ\sebastian carrero\programacion\Programacion2025\retoPYTHON\ejercicios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelson.Daza\Documents\Sebastian Carrero\Programacion2025\retoPYTHON\ejercicios\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="116">
   <si>
     <t>N°</t>
   </si>
@@ -126,254 +126,971 @@
     <t>Redondea un número decimal</t>
   </si>
   <si>
-    <t>Ejercicio de Estructuras de control #1</t>
-  </si>
-  <si>
-    <t>Ejercicio de Estructuras de control #2</t>
-  </si>
-  <si>
-    <t>Ejercicio de Estructuras de control #3</t>
-  </si>
-  <si>
-    <t>Ejercicio de Estructuras de control #4</t>
-  </si>
-  <si>
-    <t>Ejercicio de Estructuras de control #5</t>
-  </si>
-  <si>
-    <t>Ejercicio de Estructuras de control #6</t>
-  </si>
-  <si>
-    <t>Ejercicio de Estructuras de control #7</t>
-  </si>
-  <si>
-    <t>Ejercicio de Estructuras de control #8</t>
-  </si>
-  <si>
-    <t>Ejercicio de Estructuras de control #9</t>
-  </si>
-  <si>
-    <t>Ejercicio de Estructuras de control #10</t>
-  </si>
-  <si>
-    <t>Ejercicio de Estructuras de control #11</t>
-  </si>
-  <si>
-    <t>Ejercicio de Estructuras de control #12</t>
-  </si>
-  <si>
-    <t>Ejercicio de Estructuras de control #13</t>
-  </si>
-  <si>
-    <t>Ejercicio de Estructuras de control #14</t>
-  </si>
-  <si>
-    <t>Ejercicio de Estructuras de control #15</t>
-  </si>
-  <si>
-    <t>Ejercicio de Funciones y scope #1</t>
-  </si>
-  <si>
-    <t>Ejercicio de Funciones y scope #2</t>
-  </si>
-  <si>
-    <t>Ejercicio de Funciones y scope #3</t>
-  </si>
-  <si>
-    <t>Ejercicio de Funciones y scope #4</t>
-  </si>
-  <si>
-    <t>Ejercicio de Funciones y scope #5</t>
-  </si>
-  <si>
-    <t>Ejercicio de Funciones y scope #6</t>
-  </si>
-  <si>
-    <t>Ejercicio de Funciones y scope #7</t>
-  </si>
-  <si>
-    <t>Ejercicio de Funciones y scope #8</t>
-  </si>
-  <si>
-    <t>Ejercicio de Funciones y scope #9</t>
-  </si>
-  <si>
-    <t>Ejercicio de Funciones y scope #10</t>
-  </si>
-  <si>
-    <t>Ejercicio de Funciones y scope #11</t>
-  </si>
-  <si>
-    <t>Ejercicio de Funciones y scope #12</t>
-  </si>
-  <si>
-    <t>Ejercicio de Funciones y scope #13</t>
-  </si>
-  <si>
-    <t>Ejercicio de Funciones y scope #14</t>
-  </si>
-  <si>
-    <t>Ejercicio de Funciones y scope #15</t>
-  </si>
-  <si>
-    <t>Ejercicio de Listas y comprensión de listas #1</t>
-  </si>
-  <si>
-    <t>Ejercicio de Listas y comprensión de listas #2</t>
-  </si>
-  <si>
-    <t>Ejercicio de Listas y comprensión de listas #3</t>
-  </si>
-  <si>
-    <t>Ejercicio de Listas y comprensión de listas #4</t>
-  </si>
-  <si>
-    <t>Ejercicio de Listas y comprensión de listas #5</t>
-  </si>
-  <si>
-    <t>Ejercicio de Listas y comprensión de listas #6</t>
-  </si>
-  <si>
-    <t>Ejercicio de Listas y comprensión de listas #7</t>
-  </si>
-  <si>
-    <t>Ejercicio de Listas y comprensión de listas #8</t>
-  </si>
-  <si>
-    <t>Ejercicio de Listas y comprensión de listas #9</t>
-  </si>
-  <si>
-    <t>Ejercicio de Listas y comprensión de listas #10</t>
-  </si>
-  <si>
-    <t>Ejercicio de Diccionarios y sets #1</t>
-  </si>
-  <si>
-    <t>Ejercicio de Diccionarios y sets #2</t>
-  </si>
-  <si>
-    <t>Ejercicio de Diccionarios y sets #3</t>
-  </si>
-  <si>
-    <t>Ejercicio de Diccionarios y sets #4</t>
-  </si>
-  <si>
-    <t>Ejercicio de Diccionarios y sets #5</t>
-  </si>
-  <si>
-    <t>Ejercicio de Diccionarios y sets #6</t>
-  </si>
-  <si>
-    <t>Ejercicio de Diccionarios y sets #7</t>
-  </si>
-  <si>
-    <t>Ejercicio de Diccionarios y sets #8</t>
-  </si>
-  <si>
-    <t>Ejercicio de Diccionarios y sets #9</t>
-  </si>
-  <si>
-    <t>Ejercicio de Diccionarios y sets #10</t>
-  </si>
-  <si>
-    <t>Ejercicio de Manejo de errores #1</t>
-  </si>
-  <si>
-    <t>Ejercicio de Manejo de errores #2</t>
-  </si>
-  <si>
-    <t>Ejercicio de Manejo de errores #3</t>
-  </si>
-  <si>
-    <t>Ejercicio de Manejo de errores #4</t>
-  </si>
-  <si>
-    <t>Ejercicio de Manejo de errores #5</t>
-  </si>
-  <si>
-    <t>Ejercicio de Módulos y paquetes #1</t>
-  </si>
-  <si>
-    <t>Ejercicio de Módulos y paquetes #2</t>
-  </si>
-  <si>
-    <t>Ejercicio de Módulos y paquetes #3</t>
-  </si>
-  <si>
-    <t>Ejercicio de Módulos y paquetes #4</t>
-  </si>
-  <si>
-    <t>Ejercicio de Módulos y paquetes #5</t>
-  </si>
-  <si>
-    <t>Ejercicio de Lectura/escritura de archivos #1</t>
-  </si>
-  <si>
-    <t>Ejercicio de Lectura/escritura de archivos #2</t>
-  </si>
-  <si>
-    <t>Ejercicio de Lectura/escritura de archivos #3</t>
-  </si>
-  <si>
-    <t>Ejercicio de Lectura/escritura de archivos #4</t>
-  </si>
-  <si>
-    <t>Ejercicio de Lectura/escritura de archivos #5</t>
-  </si>
-  <si>
-    <t>Ejercicio de Lectura/escritura de archivos #6</t>
-  </si>
-  <si>
-    <t>Ejercicio de Lectura/escritura de archivos #7</t>
-  </si>
-  <si>
-    <t>Ejercicio de Lectura/escritura de archivos #8</t>
-  </si>
-  <si>
-    <t>Ejercicio de Lectura/escritura de archivos #9</t>
-  </si>
-  <si>
-    <t>Ejercicio de Lectura/escritura de archivos #10</t>
-  </si>
-  <si>
-    <t>Ejercicio de Manipulación básica con pandas #1</t>
-  </si>
-  <si>
-    <t>Ejercicio de Manipulación básica con pandas #2</t>
-  </si>
-  <si>
-    <t>Ejercicio de Manipulación básica con pandas #3</t>
-  </si>
-  <si>
-    <t>Ejercicio de Manipulación básica con pandas #4</t>
-  </si>
-  <si>
-    <t>Ejercicio de Manipulación básica con pandas #5</t>
-  </si>
-  <si>
-    <t>Ejercicio de Manipulación básica con pandas #6</t>
-  </si>
-  <si>
-    <t>Ejercicio de Manipulación básica con pandas #7</t>
-  </si>
-  <si>
-    <t>Ejercicio de Manipulación básica con pandas #8</t>
-  </si>
-  <si>
-    <t>Ejercicio de Manipulación básica con pandas #9</t>
-  </si>
-  <si>
-    <t>Ejercicio de Manipulación básica con pandas #10</t>
-  </si>
-  <si>
     <t>si</t>
+  </si>
+  <si>
+    <t>Solicita un número al usuario y determina si es positivo, negativo o cero.</t>
+  </si>
+  <si>
+    <t>Pide la edad de una persona y determina si puede votar (mayor o igual a 18 años).</t>
+  </si>
+  <si>
+    <t>Solicita tres números y muestra cuál es el mayor usando condicionales.</t>
+  </si>
+  <si>
+    <t>Pide un número del 1 al 7 y muestra el día de la semana correspondiente (1=Lunes, ..., 7=Domingo).</t>
+  </si>
+  <si>
+    <t>Escribe un programa que determine si un año es bisiesto.</t>
+  </si>
+  <si>
+    <t>Pide un número al usuario y determina si es par o impar.</t>
+  </si>
+  <si>
+    <t>Solicita una contraseña al usuario y valida si coincide con una clave predefinida.</t>
+  </si>
+  <si>
+    <t>Crea un menú con tres opciones, elige una y realiza una acción diferente según la opción seleccionada.</t>
+  </si>
+  <si>
+    <t>Pide un número entero y muestra todos los números desde 1 hasta ese número usando un bucle.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Muestra la tabla de multiplicar de un número dado por el usuario, usando un bucle </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Solicita una lista de números al usuario (separados por coma) y muestra solo los números pares.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Escribe un programa que sume todos los números del 1 al 100 usando un bucle </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>while</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Crea un programa que cuente cuántas vocales hay en una cadena ingresada por el usuario.</t>
+  </si>
+  <si>
+    <t>Solicita un número entero y determina si es primo.</t>
+  </si>
+  <si>
+    <t>Crea una función que reciba un número y devuelva su cuadrado.</t>
+  </si>
+  <si>
+    <t>Define una función que reciba dos números y retorne su suma.</t>
+  </si>
+  <si>
+    <t>Escribe una función que reciba una lista de números y devuelva la suma de todos.</t>
+  </si>
+  <si>
+    <t>Crea una función que verifique si una palabra es un palíndromo (se lee igual al derecho y al revés).</t>
+  </si>
+  <si>
+    <t>Define una función que reciba una lista de números y devuelva el mayor.</t>
+  </si>
+  <si>
+    <t>Crea una función que reciba una temperatura en Celsius y la convierta a Fahrenheit.</t>
+  </si>
+  <si>
+    <t>Escribe una función que cuente cuántas veces aparece una letra en una frase.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Crea una función que reciba un número y devuelva </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>True</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> si es par y </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>False</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> si es impar.</t>
+    </r>
+  </si>
+  <si>
+    <t>Define una función con un parámetro opcional. Si el parámetro no se pasa, que imprima "Parámetro no recibido".</t>
+  </si>
+  <si>
+    <t>Crea una función que reciba el nombre y la edad de una persona y devuelva un saludo personalizado.</t>
+  </si>
+  <si>
+    <t>Escribe una función que calcule el factorial de un número (usa recursión).</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Crea una función </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>login</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> que reciba un usuario y una contraseña y verifique si coinciden con valores predefinidos.</t>
+    </r>
+  </si>
+  <si>
+    <t>Define una variable global y otra local con el mismo nombre. Muestra el valor de ambas dentro y fuera de una función.</t>
+  </si>
+  <si>
+    <t>Crea una función que reciba un número entero y devuelva una lista con todos los números primos menores a él.</t>
+  </si>
+  <si>
+    <t>Define una función que determine si un año es bisiesto (reutiliza la lógica del ejercicio 25).</t>
+  </si>
+  <si>
+    <t>Crea una lista con 10 números ingresados por el usuario y muestra la lista invertida.</t>
+  </si>
+  <si>
+    <t>Solicita al usuario una lista de palabras y muestra solo las que tengan más de 5 letras.</t>
+  </si>
+  <si>
+    <t>Usa comprensión de listas para generar una lista de los cuadrados de los números del 1 al 10.</t>
+  </si>
+  <si>
+    <t>Dada una lista de nombres, crea una nueva lista que contenga solo los nombres que comienzan con la letra "A".</t>
+  </si>
+  <si>
+    <t>Crea una lista de números del 1 al 20 y usa comprensión de listas para generar una lista de los múltiplos de 3.</t>
+  </si>
+  <si>
+    <t>Pide al usuario 5 notas y guárdalas en una lista. Luego, muestra la nota mayor, menor y el promedio.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Dada una lista de números, crea una nueva lista que contenga </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>True</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> si el número es par y </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>False</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> si es impar.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Genera una lista de tuplas </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>(número, cuadrado)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> para los números del 1 al 10 usando comprensión de listas.</t>
+    </r>
+  </si>
+  <si>
+    <t>Solicita al usuario una lista de palabras y muestra otra lista con esas palabras en mayúsculas.</t>
+  </si>
+  <si>
+    <t>Elimina los elementos duplicados de una lista ingresada por el usuario y muestra la nueva lista sin repeticiones.</t>
+  </si>
+  <si>
+    <t>Solicita al usuario ingresar 5 pares clave-valor y guárdalos en un diccionario. Luego, muestra el diccionario completo.</t>
+  </si>
+  <si>
+    <t>Dado un diccionario de productos y precios, permite al usuario consultar el precio ingresando el nombre del producto.</t>
+  </si>
+  <si>
+    <t>Agrega una nueva entrada a un diccionario ya creado y muestra el resultado.</t>
+  </si>
+  <si>
+    <t>Recorre un diccionario e imprime cada clave junto con su valor.</t>
+  </si>
+  <si>
+    <t>Dado un diccionario con nombres y notas, muestra la nota promedio de todos los estudiantes.</t>
+  </si>
+  <si>
+    <t>Crea un set con 5 elementos ingresados por el usuario y muestra cuántos elementos únicos hay.</t>
+  </si>
+  <si>
+    <t>Dadas dos listas, crea un set con los elementos comunes a ambas.</t>
+  </si>
+  <si>
+    <t>Usa un set para eliminar los elementos duplicados de una lista ingresada por el usuario.</t>
+  </si>
+  <si>
+    <t>Pide al usuario dos sets y muestra la unión, intersección y diferencia entre ellos.</t>
+  </si>
+  <si>
+    <t>Solicita al usuario ingresar un número entero. Si el valor ingresado no es un número, muestra un mensaje de error personalizado.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Crea un programa que abra un archivo inexistente con </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>open()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> y maneje la excepción para mostrar un mensaje que diga "Archivo no encontrado".</t>
+    </r>
+  </si>
+  <si>
+    <t>Pide al usuario una posición y accede a un elemento de una lista. Si la posición no existe, captura el error y muestra un mensaje adecuado.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Utiliza el módulo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>math</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> para calcular la raíz cuadrada de un número ingresado por el usuario.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Usa el módulo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>random</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> para simular el lanzamiento de un dado de seis caras.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Crea un programa que cree un archivo de texto llamado </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>saludo.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> y escriba la frase "Hola, mundo".</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Escribe un programa que lea el contenido del archivo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>saludo.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> y lo muestre en pantalla.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Escribe un programa que permita al usuario ingresar varias líneas de texto y las guarde en un archivo llamado </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>notas.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Crea un programa que cuente cuántas líneas tiene el archivo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>notas.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Escribe un programa que lea un archivo línea por línea y las muestre con su número de línea correspondiente.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Modifica el archivo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>notas.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> añadiendo una nueva línea sin borrar su contenido anterior.</t>
+    </r>
+  </si>
+  <si>
+    <t>Escribe un programa que lea un archivo y muestre cuántas veces aparece una palabra específica.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Crea un programa que copie el contenido de un archivo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>origen.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> a otro llamado </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>copia.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Crea un archivo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>numeros.txt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> que contenga una lista de números (uno por línea). Luego, crea otro archivo donde se guarde el doble de cada número.</t>
+    </r>
+  </si>
+  <si>
+    <t>Escribe un programa que elimine un archivo si el usuario confirma que desea borrarlo.</t>
+  </si>
+  <si>
+    <t>Crea un DataFrame a partir de un diccionario con los nombres y edades de 5 personas.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Lee un archivo CSV llamado </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>personas.csv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> que contenga columnas como nombre, edad y ciudad.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Muestra las primeras 5 filas del DataFrame cargado desde </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>personas.csv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Muestra el resumen estadístico de las columnas numéricas del DataFrame.</t>
+  </si>
+  <si>
+    <t>Filtra el DataFrame para mostrar solo las personas mayores de 30 años.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Agrega una nueva columna al DataFrame llamada </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>año_nacimiento</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> calculada a partir de la edad.</t>
+    </r>
+  </si>
+  <si>
+    <t>Ordena el DataFrame por la columna edad de manera descendente.</t>
+  </si>
+  <si>
+    <t>Agrupa el DataFrame por ciudad y calcula la edad promedio en cada ciudad.</t>
+  </si>
+  <si>
+    <t>Elimina las filas que contengan valores nulos (NaN) en cualquier columna.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Guarda el DataFrame resultante en un nuevo archivo CSV llamado </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>resultado.csv</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Simula un intento de inicio de sesión con un máximo de 3 intentos. Si el usuario ingresa 
+la contraseña correcta antes de los 3 intentos, mostrar "Acceso permitido".</t>
+  </si>
+  <si>
+    <t>Crea un diccionario donde las claves sean nombres de personas y los valores sus edades. Luego, 
+imprime la edad de una persona consultando por su nombre.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Crea un programa que solicite dos números al usuario e intente dividirlos. Usa un bloque </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>try-except</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> para manejar el caso en que 
+el segundo número sea cero.</t>
+    </r>
+  </si>
+  <si>
+    <t>Escribe un programa que combine múltiples excepciones: intenta convertir un dato a entero, dividir entre cero, y acceder a una posición 
+inexistente en una lista. Captura cada tipo de error por separado y muestra un mensaje específico para cada caso.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Crea un módulo llamado </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>saludos.py</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> que contenga una función </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>saludar(nombre)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> que imprima un saludo personalizado. 
+Luego, impórtalo en un archivo principal y úsalo.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Crea un paquete llamado </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>matematica</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> que tenga un módulo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>operaciones.py</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> con funciones para sumar, restar y multiplicar. 
+Usa este paquete desde otro archivo.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Crea un archivo Python que importe funciones específicas de otro archivo (por ejemplo, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>from operaciones import sumar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) y demuéstralo con 
+un ejemplo práctico.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -388,6 +1105,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -425,10 +1147,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -736,19 +1462,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="64.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="129.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -765,7 +1491,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -776,10 +1502,10 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -790,10 +1516,10 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -804,10 +1530,10 @@
         <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -818,10 +1544,10 @@
         <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -832,10 +1558,10 @@
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -846,10 +1572,10 @@
         <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>7</v>
       </c>
@@ -860,10 +1586,10 @@
         <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>8</v>
       </c>
@@ -874,10 +1600,10 @@
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>9</v>
       </c>
@@ -888,10 +1614,10 @@
         <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>10</v>
       </c>
@@ -902,10 +1628,10 @@
         <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>11</v>
       </c>
@@ -916,10 +1642,10 @@
         <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>12</v>
       </c>
@@ -930,10 +1656,10 @@
         <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>13</v>
       </c>
@@ -944,10 +1670,10 @@
         <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>14</v>
       </c>
@@ -958,10 +1684,10 @@
         <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>15</v>
       </c>
@@ -971,8 +1697,11 @@
       <c r="C16" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>16</v>
       </c>
@@ -982,8 +1711,11 @@
       <c r="C17" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>17</v>
       </c>
@@ -993,8 +1725,11 @@
       <c r="C18" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1004,8 +1739,11 @@
       <c r="C19" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1015,8 +1753,11 @@
       <c r="C20" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1026,118 +1767,151 @@
       <c r="C21" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
       </c>
-      <c r="C22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
       </c>
-      <c r="C23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
       </c>
-      <c r="C24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
       </c>
-      <c r="C25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
       </c>
-      <c r="C26" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
       </c>
-      <c r="C27" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
       </c>
-      <c r="C28" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
       </c>
-      <c r="C29" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
       </c>
-      <c r="C30" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>7</v>
       </c>
-      <c r="C31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1145,54 +1919,54 @@
         <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>7</v>
       </c>
-      <c r="C33" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>7</v>
       </c>
-      <c r="C34" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>7</v>
       </c>
-      <c r="C35" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="30">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>7</v>
       </c>
-      <c r="C36" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1203,712 +1977,712 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>8</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>8</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>8</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>8</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>8</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>8</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>8</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>8</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
         <v>8</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
         <v>8</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>8</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>8</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>8</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
         <v>8</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>9</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
         <v>9</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
         <v>9</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
         <v>9</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
         <v>9</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
         <v>9</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
         <v>9</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
         <v>9</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
         <v>9</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
         <v>9</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" ht="30">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" t="s">
         <v>10</v>
       </c>
-      <c r="C62" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C62" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
         <v>10</v>
       </c>
-      <c r="C63" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C63" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" t="s">
         <v>10</v>
       </c>
-      <c r="C64" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C64" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" t="s">
         <v>10</v>
       </c>
-      <c r="C65" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C65" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" t="s">
         <v>10</v>
       </c>
-      <c r="C66" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C66" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" t="s">
         <v>10</v>
       </c>
-      <c r="C67" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C67" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" t="s">
         <v>10</v>
       </c>
-      <c r="C68" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C68" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" t="s">
         <v>10</v>
       </c>
-      <c r="C69" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C69" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70" t="s">
         <v>10</v>
       </c>
-      <c r="C70" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C70" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" t="s">
         <v>10</v>
       </c>
-      <c r="C71" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C71" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="30">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72" t="s">
         <v>11</v>
       </c>
-      <c r="C72" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C72" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" t="s">
         <v>11</v>
       </c>
-      <c r="C73" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C73" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74" t="s">
         <v>11</v>
       </c>
-      <c r="C74" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C74" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" t="s">
         <v>11</v>
       </c>
-      <c r="C75" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C75" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="30">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76" t="s">
         <v>11</v>
       </c>
-      <c r="C76" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C76" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="30">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77" t="s">
         <v>12</v>
       </c>
-      <c r="C77" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C77" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="30">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78" t="s">
         <v>12</v>
       </c>
-      <c r="C78" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C78" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
       <c r="A79">
         <v>78</v>
       </c>
       <c r="B79" t="s">
         <v>12</v>
       </c>
-      <c r="C79" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C79" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
       <c r="A80">
         <v>79</v>
       </c>
       <c r="B80" t="s">
         <v>12</v>
       </c>
-      <c r="C80" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C80" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="30">
       <c r="A81">
         <v>80</v>
       </c>
       <c r="B81" t="s">
         <v>12</v>
       </c>
-      <c r="C81" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C81" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
       <c r="A82">
         <v>81</v>
       </c>
       <c r="B82" t="s">
         <v>13</v>
       </c>
-      <c r="C82" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C82" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83" t="s">
         <v>13</v>
       </c>
-      <c r="C83" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C83" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
       <c r="A84">
         <v>83</v>
       </c>
       <c r="B84" t="s">
         <v>13</v>
       </c>
-      <c r="C84" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C84" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
       <c r="A85">
         <v>84</v>
       </c>
       <c r="B85" t="s">
         <v>13</v>
       </c>
-      <c r="C85" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C85" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
       <c r="A86">
         <v>85</v>
       </c>
       <c r="B86" t="s">
         <v>13</v>
       </c>
-      <c r="C86" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C86" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
       <c r="A87">
         <v>86</v>
       </c>
       <c r="B87" t="s">
         <v>13</v>
       </c>
-      <c r="C87" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C87" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
       <c r="A88">
         <v>87</v>
       </c>
       <c r="B88" t="s">
         <v>13</v>
       </c>
-      <c r="C88" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C88" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
       <c r="A89">
         <v>88</v>
       </c>
       <c r="B89" t="s">
         <v>13</v>
       </c>
-      <c r="C89" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C89" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
       <c r="A90">
         <v>89</v>
       </c>
       <c r="B90" t="s">
         <v>13</v>
       </c>
-      <c r="C90" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C90" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
       <c r="A91">
         <v>90</v>
       </c>
       <c r="B91" t="s">
         <v>13</v>
       </c>
-      <c r="C91" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C91" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
       <c r="A92">
         <v>91</v>
       </c>
       <c r="B92" t="s">
         <v>14</v>
       </c>
-      <c r="C92" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C92" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
       <c r="A93">
         <v>92</v>
       </c>
       <c r="B93" t="s">
         <v>14</v>
       </c>
-      <c r="C93" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C93" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
       <c r="A94">
         <v>93</v>
       </c>
       <c r="B94" t="s">
         <v>14</v>
       </c>
-      <c r="C94" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C94" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
       <c r="A95">
         <v>94</v>
       </c>
       <c r="B95" t="s">
         <v>14</v>
       </c>
-      <c r="C95" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C95" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
       <c r="A96">
         <v>95</v>
       </c>
       <c r="B96" t="s">
         <v>14</v>
       </c>
-      <c r="C96" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C96" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
       <c r="A97">
         <v>96</v>
       </c>
       <c r="B97" t="s">
         <v>14</v>
       </c>
-      <c r="C97" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C97" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
       <c r="A98">
         <v>97</v>
       </c>
       <c r="B98" t="s">
         <v>14</v>
       </c>
-      <c r="C98" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C98" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
       <c r="A99">
         <v>98</v>
       </c>
       <c r="B99" t="s">
         <v>14</v>
       </c>
-      <c r="C99" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C99" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
       <c r="A100">
         <v>99</v>
       </c>
       <c r="B100" t="s">
         <v>14</v>
       </c>
-      <c r="C100" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C100" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
       <c r="A101">
         <v>100</v>
       </c>
       <c r="B101" t="s">
         <v>14</v>
       </c>
-      <c r="C101" t="s">
-        <v>114</v>
+      <c r="C101" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ejercicio 33 al 36
</commit_message>
<xml_diff>
--- a/retoPYTHON/ejercicios/100_ejercicios_python_para_ingeniero_datos.xlsx
+++ b/retoPYTHON/ejercicios/100_ejercicios_python_para_ingeniero_datos.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="116">
   <si>
     <t>N°</t>
   </si>
@@ -1462,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1963,6 +1963,9 @@
       <c r="C35" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="D35" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="36" spans="1:4" ht="30">
       <c r="A36">
@@ -1973,6 +1976,9 @@
       </c>
       <c r="C36" s="3" t="s">
         <v>109</v>
+      </c>
+      <c r="D36" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:4">

</xml_diff>

<commit_message>
ejercicios python del 38 al 40
</commit_message>
<xml_diff>
--- a/retoPYTHON/ejercicios/100_ejercicios_python_para_ingeniero_datos.xlsx
+++ b/retoPYTHON/ejercicios/100_ejercicios_python_para_ingeniero_datos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelson.Daza\Documents\Sebastian Carrero\Programacion2025\retoPYTHON\ejercicios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OD\OneDrive - TI\Documentos\Sebastian Carrero\Programacion2025\retoPYTHON\ejercicios\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="116">
   <si>
     <t>N°</t>
   </si>
@@ -1463,7 +1463,7 @@
   <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2019,6 +2019,9 @@
       <c r="C39" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="D39" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40">
@@ -2030,6 +2033,9 @@
       <c r="C40" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="D40" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41">
@@ -2040,6 +2046,9 @@
       </c>
       <c r="C41" s="2" t="s">
         <v>54</v>
+      </c>
+      <c r="D41" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:4">

</xml_diff>

<commit_message>
ejercicio 43 a 48
</commit_message>
<xml_diff>
--- a/retoPYTHON/ejercicios/100_ejercicios_python_para_ingeniero_datos.xlsx
+++ b/retoPYTHON/ejercicios/100_ejercicios_python_para_ingeniero_datos.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="116">
   <si>
     <t>N°</t>
   </si>
@@ -1462,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2089,6 +2089,9 @@
       <c r="C44" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="D44" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45">
@@ -2100,6 +2103,9 @@
       <c r="C45" s="2" t="s">
         <v>58</v>
       </c>
+      <c r="D45" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46">
@@ -2111,6 +2117,9 @@
       <c r="C46" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="D46" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47">
@@ -2122,6 +2131,9 @@
       <c r="C47" s="2" t="s">
         <v>60</v>
       </c>
+      <c r="D47" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48">
@@ -2133,8 +2145,11 @@
       <c r="C48" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
+      <c r="D48" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2144,8 +2159,11 @@
       <c r="C49" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="50" spans="1:3">
+      <c r="D49" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2156,7 +2174,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:4">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2167,7 +2185,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:4">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2178,7 +2196,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:4">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2189,7 +2207,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:4">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2200,7 +2218,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:4">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2211,7 +2229,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:4">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2222,7 +2240,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:4">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2233,7 +2251,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:4">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2244,7 +2262,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:4">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2255,7 +2273,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:4">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2266,7 +2284,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:4">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2277,7 +2295,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="30">
+    <row r="62" spans="1:4" ht="30">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2288,7 +2306,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:4">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2299,7 +2317,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:4">
       <c r="A64">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
ejercicio 49 al 51
</commit_message>
<xml_diff>
--- a/retoPYTHON/ejercicios/100_ejercicios_python_para_ingeniero_datos.xlsx
+++ b/retoPYTHON/ejercicios/100_ejercicios_python_para_ingeniero_datos.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="116">
   <si>
     <t>N°</t>
   </si>
@@ -1463,7 +1463,7 @@
   <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2173,6 +2173,9 @@
       <c r="C50" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="D50" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51">
@@ -2184,6 +2187,9 @@
       <c r="C51" s="2" t="s">
         <v>64</v>
       </c>
+      <c r="D51" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52">
@@ -2194,6 +2200,9 @@
       </c>
       <c r="C52" s="2" t="s">
         <v>65</v>
+      </c>
+      <c r="D52" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="53" spans="1:4">

</xml_diff>

<commit_message>
Ejercicios 52 al 59
</commit_message>
<xml_diff>
--- a/retoPYTHON/ejercicios/100_ejercicios_python_para_ingeniero_datos.xlsx
+++ b/retoPYTHON/ejercicios/100_ejercicios_python_para_ingeniero_datos.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="116">
   <si>
     <t>N°</t>
   </si>
@@ -1462,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2215,6 +2215,9 @@
       <c r="C53" s="2" t="s">
         <v>66</v>
       </c>
+      <c r="D53" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54">
@@ -2226,6 +2229,9 @@
       <c r="C54" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="D54" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55">
@@ -2237,6 +2243,9 @@
       <c r="C55" s="2" t="s">
         <v>68</v>
       </c>
+      <c r="D55" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56">
@@ -2248,6 +2257,9 @@
       <c r="C56" s="2" t="s">
         <v>69</v>
       </c>
+      <c r="D56" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57">
@@ -2259,6 +2271,9 @@
       <c r="C57" s="2" t="s">
         <v>70</v>
       </c>
+      <c r="D57" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58">
@@ -2270,6 +2285,9 @@
       <c r="C58" s="2" t="s">
         <v>71</v>
       </c>
+      <c r="D58" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59">
@@ -2281,6 +2299,9 @@
       <c r="C59" s="2" t="s">
         <v>72</v>
       </c>
+      <c r="D59" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60">
@@ -2291,6 +2312,9 @@
       </c>
       <c r="C60" s="2" t="s">
         <v>73</v>
+      </c>
+      <c r="D60" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="61" spans="1:4">

</xml_diff>

<commit_message>
ejercicios 66 al 68
</commit_message>
<xml_diff>
--- a/retoPYTHON/ejercicios/100_ejercicios_python_para_ingeniero_datos.xlsx
+++ b/retoPYTHON/ejercicios/100_ejercicios_python_para_ingeniero_datos.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="116">
   <si>
     <t>N°</t>
   </si>
@@ -1462,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2411,6 +2411,9 @@
       <c r="C67" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="D67" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68">
@@ -2421,6 +2424,9 @@
       </c>
       <c r="C68" s="2" t="s">
         <v>80</v>
+      </c>
+      <c r="D68" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="69" spans="1:4">

</xml_diff>

<commit_message>
ejercicio 68 y 69
</commit_message>
<xml_diff>
--- a/retoPYTHON/ejercicios/100_ejercicios_python_para_ingeniero_datos.xlsx
+++ b/retoPYTHON/ejercicios/100_ejercicios_python_para_ingeniero_datos.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="116">
   <si>
     <t>N°</t>
   </si>
@@ -1462,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2439,6 +2439,9 @@
       <c r="C69" s="2" t="s">
         <v>81</v>
       </c>
+      <c r="D69" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70">
@@ -2449,6 +2452,9 @@
       </c>
       <c r="C70" s="2" t="s">
         <v>82</v>
+      </c>
+      <c r="D70" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="71" spans="1:4">

</xml_diff>